<commit_message>
Recompiled CAC, AIM, Custom Units/Voices. - Fixed LOS colours. Updated store control file for testing.
</commit_message>
<xml_diff>
--- a/vfProcGenStores/res/test-xlrp-store-content.xlsx
+++ b/vfProcGenStores/res/test-xlrp-store-content.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephen Weistra\gitrepos\vfBattleTechMod-Core\vfBattleTechMod-ProcGenStores-Test\res\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Games\Steam\steamapps\common\BATTLETECH\Mods\vfProcGenStores\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E39DB21-7E96-4038-B20C-FBFFBDA3561F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B4C5F05-4BD2-4A07-85CD-CFA2799D8B70}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4275" yWindow="-21720" windowWidth="38640" windowHeight="21240" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="1830" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UpgradeDef" sheetId="1" r:id="rId1"/>
@@ -7514,9 +7514,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J135"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="48.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="97.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="142.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
@@ -7598,7 +7612,7 @@
         <v>11</v>
       </c>
       <c r="G4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="H4" t="s">
         <v>11</v>
@@ -7618,7 +7632,7 @@
         <v>11</v>
       </c>
       <c r="G5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="H5" t="s">
         <v>11</v>
@@ -7638,7 +7652,7 @@
         <v>11</v>
       </c>
       <c r="G6" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="H6" t="s">
         <v>11</v>
@@ -7658,7 +7672,7 @@
         <v>11</v>
       </c>
       <c r="G7" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="H7" t="s">
         <v>11</v>
@@ -7678,7 +7692,7 @@
         <v>11</v>
       </c>
       <c r="G8" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="H8" t="s">
         <v>11</v>
@@ -7698,7 +7712,7 @@
         <v>11</v>
       </c>
       <c r="G9" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="H9" t="s">
         <v>11</v>
@@ -7718,7 +7732,7 @@
         <v>11</v>
       </c>
       <c r="G10" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="H10" t="s">
         <v>11</v>
@@ -7738,7 +7752,7 @@
         <v>11</v>
       </c>
       <c r="G11" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="H11" t="s">
         <v>11</v>
@@ -7778,7 +7792,7 @@
         <v>11</v>
       </c>
       <c r="G13" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="H13" t="s">
         <v>11</v>
@@ -7838,7 +7852,7 @@
         <v>11</v>
       </c>
       <c r="G16" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="H16" t="s">
         <v>11</v>
@@ -7858,7 +7872,7 @@
         <v>11</v>
       </c>
       <c r="G17" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="H17" t="s">
         <v>11</v>
@@ -7878,7 +7892,7 @@
         <v>11</v>
       </c>
       <c r="G18" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="H18" t="s">
         <v>11</v>
@@ -7898,7 +7912,7 @@
         <v>11</v>
       </c>
       <c r="G19" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="H19" t="s">
         <v>11</v>
@@ -7938,7 +7952,7 @@
         <v>11</v>
       </c>
       <c r="G21" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="H21" t="s">
         <v>11</v>
@@ -10242,6 +10256,10 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="7" max="7" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="73.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
@@ -10964,7 +10982,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J532"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
@@ -21629,8 +21647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C108" sqref="C108"/>
     </sheetView>
   </sheetViews>
@@ -23850,7 +23868,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
@@ -23894,7 +23914,7 @@
         <v>11</v>
       </c>
       <c r="G2" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="H2" t="s">
         <v>11</v>
@@ -23954,7 +23974,7 @@
         <v>11</v>
       </c>
       <c r="G5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H5" t="s">
         <v>11</v>
@@ -23995,9 +24015,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J224"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A196" workbookViewId="0">
+      <selection activeCell="G224" sqref="G224"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="7" max="7" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.28515625" customWidth="1"/>
+    <col min="9" max="9" width="19.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
@@ -24919,7 +24946,7 @@
         <v>11</v>
       </c>
       <c r="G46" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H46" t="s">
         <v>11</v>
@@ -24939,7 +24966,7 @@
         <v>11</v>
       </c>
       <c r="G47" t="s">
-        <v>57</v>
+        <v>90</v>
       </c>
       <c r="H47" t="s">
         <v>11</v>
@@ -24959,7 +24986,7 @@
         <v>11</v>
       </c>
       <c r="G48" t="s">
-        <v>57</v>
+        <v>90</v>
       </c>
       <c r="H48" t="s">
         <v>11</v>
@@ -24979,7 +25006,7 @@
         <v>11</v>
       </c>
       <c r="G49" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H49" t="s">
         <v>11</v>
@@ -24999,7 +25026,7 @@
         <v>11</v>
       </c>
       <c r="G50" t="s">
-        <v>57</v>
+        <v>90</v>
       </c>
       <c r="H50" t="s">
         <v>11</v>
@@ -25019,7 +25046,7 @@
         <v>11</v>
       </c>
       <c r="G51" t="s">
-        <v>57</v>
+        <v>90</v>
       </c>
       <c r="H51" t="s">
         <v>11</v>
@@ -25039,7 +25066,7 @@
         <v>11</v>
       </c>
       <c r="G52" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H52" t="s">
         <v>11</v>
@@ -25059,7 +25086,7 @@
         <v>11</v>
       </c>
       <c r="G53" t="s">
-        <v>57</v>
+        <v>90</v>
       </c>
       <c r="H53" t="s">
         <v>11</v>
@@ -25079,7 +25106,7 @@
         <v>11</v>
       </c>
       <c r="G54" t="s">
-        <v>57</v>
+        <v>90</v>
       </c>
       <c r="H54" t="s">
         <v>11</v>
@@ -25099,7 +25126,7 @@
         <v>11</v>
       </c>
       <c r="G55" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H55" t="s">
         <v>11</v>
@@ -25119,7 +25146,7 @@
         <v>11</v>
       </c>
       <c r="G56" t="s">
-        <v>57</v>
+        <v>90</v>
       </c>
       <c r="H56" t="s">
         <v>11</v>
@@ -25139,7 +25166,7 @@
         <v>11</v>
       </c>
       <c r="G57" t="s">
-        <v>57</v>
+        <v>90</v>
       </c>
       <c r="H57" t="s">
         <v>11</v>
@@ -25159,7 +25186,7 @@
         <v>11</v>
       </c>
       <c r="G58" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H58" t="s">
         <v>11</v>
@@ -25179,7 +25206,7 @@
         <v>11</v>
       </c>
       <c r="G59" t="s">
-        <v>57</v>
+        <v>90</v>
       </c>
       <c r="H59" t="s">
         <v>11</v>
@@ -25199,7 +25226,7 @@
         <v>11</v>
       </c>
       <c r="G60" t="s">
-        <v>57</v>
+        <v>90</v>
       </c>
       <c r="H60" t="s">
         <v>11</v>
@@ -25219,7 +25246,7 @@
         <v>11</v>
       </c>
       <c r="G61" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H61" t="s">
         <v>11</v>
@@ -25239,7 +25266,7 @@
         <v>11</v>
       </c>
       <c r="G62" t="s">
-        <v>57</v>
+        <v>90</v>
       </c>
       <c r="H62" t="s">
         <v>11</v>
@@ -25259,7 +25286,7 @@
         <v>11</v>
       </c>
       <c r="G63" t="s">
-        <v>57</v>
+        <v>90</v>
       </c>
       <c r="H63" t="s">
         <v>11</v>
@@ -25279,7 +25306,7 @@
         <v>11</v>
       </c>
       <c r="G64" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H64" t="s">
         <v>11</v>
@@ -25299,7 +25326,7 @@
         <v>11</v>
       </c>
       <c r="G65" t="s">
-        <v>57</v>
+        <v>90</v>
       </c>
       <c r="H65" t="s">
         <v>11</v>
@@ -25319,7 +25346,7 @@
         <v>11</v>
       </c>
       <c r="G66" t="s">
-        <v>57</v>
+        <v>90</v>
       </c>
       <c r="H66" t="s">
         <v>11</v>
@@ -25379,7 +25406,7 @@
         <v>11</v>
       </c>
       <c r="G69" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H69" t="s">
         <v>11</v>
@@ -25399,7 +25426,7 @@
         <v>11</v>
       </c>
       <c r="G70" t="s">
-        <v>57</v>
+        <v>90</v>
       </c>
       <c r="H70" t="s">
         <v>11</v>
@@ -25419,7 +25446,7 @@
         <v>11</v>
       </c>
       <c r="G71" t="s">
-        <v>57</v>
+        <v>90</v>
       </c>
       <c r="H71" t="s">
         <v>11</v>
@@ -25439,7 +25466,7 @@
         <v>11</v>
       </c>
       <c r="G72" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H72" t="s">
         <v>11</v>
@@ -25459,7 +25486,7 @@
         <v>11</v>
       </c>
       <c r="G73" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H73" t="s">
         <v>11</v>
@@ -25479,7 +25506,7 @@
         <v>11</v>
       </c>
       <c r="G74" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H74" t="s">
         <v>11</v>
@@ -25499,7 +25526,7 @@
         <v>11</v>
       </c>
       <c r="G75" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="H75" t="s">
         <v>11</v>
@@ -25599,7 +25626,7 @@
         <v>11</v>
       </c>
       <c r="G80" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="H80" t="s">
         <v>11</v>
@@ -25699,7 +25726,7 @@
         <v>11</v>
       </c>
       <c r="G85" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H85" t="s">
         <v>11</v>
@@ -25719,7 +25746,7 @@
         <v>11</v>
       </c>
       <c r="G86" t="s">
-        <v>57</v>
+        <v>90</v>
       </c>
       <c r="H86" t="s">
         <v>11</v>
@@ -25739,7 +25766,7 @@
         <v>11</v>
       </c>
       <c r="G87" t="s">
-        <v>57</v>
+        <v>90</v>
       </c>
       <c r="H87" t="s">
         <v>11</v>
@@ -25759,7 +25786,7 @@
         <v>11</v>
       </c>
       <c r="G88" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="H88" t="s">
         <v>11</v>
@@ -25779,7 +25806,7 @@
         <v>11</v>
       </c>
       <c r="G89" t="s">
-        <v>73</v>
+        <v>12</v>
       </c>
       <c r="H89" t="s">
         <v>11</v>
@@ -27479,7 +27506,7 @@
         <v>11</v>
       </c>
       <c r="G174" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="H174" t="s">
         <v>11</v>
@@ -27539,7 +27566,7 @@
         <v>11</v>
       </c>
       <c r="G177" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H177" t="s">
         <v>11</v>
@@ -27559,7 +27586,7 @@
         <v>11</v>
       </c>
       <c r="G178" t="s">
-        <v>57</v>
+        <v>90</v>
       </c>
       <c r="H178" t="s">
         <v>11</v>
@@ -27579,7 +27606,7 @@
         <v>11</v>
       </c>
       <c r="G179" t="s">
-        <v>57</v>
+        <v>90</v>
       </c>
       <c r="H179" t="s">
         <v>11</v>
@@ -27839,7 +27866,7 @@
         <v>11</v>
       </c>
       <c r="G192" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H192" t="s">
         <v>11</v>
@@ -27859,7 +27886,7 @@
         <v>11</v>
       </c>
       <c r="G193" t="s">
-        <v>57</v>
+        <v>90</v>
       </c>
       <c r="H193" t="s">
         <v>11</v>
@@ -27879,7 +27906,7 @@
         <v>11</v>
       </c>
       <c r="G194" t="s">
-        <v>57</v>
+        <v>90</v>
       </c>
       <c r="H194" t="s">
         <v>11</v>
@@ -27899,7 +27926,7 @@
         <v>11</v>
       </c>
       <c r="G195" t="s">
-        <v>57</v>
+        <v>90</v>
       </c>
       <c r="H195" t="s">
         <v>11</v>
@@ -27919,7 +27946,7 @@
         <v>11</v>
       </c>
       <c r="G196" t="s">
-        <v>57</v>
+        <v>90</v>
       </c>
       <c r="H196" t="s">
         <v>11</v>
@@ -27939,7 +27966,7 @@
         <v>11</v>
       </c>
       <c r="G197" t="s">
-        <v>57</v>
+        <v>90</v>
       </c>
       <c r="H197" t="s">
         <v>11</v>
@@ -27959,7 +27986,7 @@
         <v>11</v>
       </c>
       <c r="G198" t="s">
-        <v>57</v>
+        <v>90</v>
       </c>
       <c r="H198" t="s">
         <v>11</v>
@@ -27979,7 +28006,7 @@
         <v>11</v>
       </c>
       <c r="G199" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="H199" t="s">
         <v>11</v>
@@ -28419,7 +28446,7 @@
         <v>11</v>
       </c>
       <c r="G221" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="H221" t="s">
         <v>11</v>
@@ -28439,7 +28466,7 @@
         <v>11</v>
       </c>
       <c r="G222" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H222" t="s">
         <v>11</v>
@@ -28459,7 +28486,7 @@
         <v>11</v>
       </c>
       <c r="G223" t="s">
-        <v>57</v>
+        <v>90</v>
       </c>
       <c r="H223" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Couple more sanity settings...
</commit_message>
<xml_diff>
--- a/vfProcGenStores/res/test-xlrp-store-content.xlsx
+++ b/vfProcGenStores/res/test-xlrp-store-content.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephen Weistra\gitrepos\XLRP-Complete\vfProcGenStores\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFFAF9EE-F1E1-4B46-A12D-E29CD3CA7205}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7BB5BC1-D953-4DED-A0E6-C9548B039C82}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4275" yWindow="-21720" windowWidth="38640" windowHeight="21240" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-4275" yWindow="-21720" windowWidth="38640" windowHeight="21240" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UpgradeDef" sheetId="1" r:id="rId1"/>
@@ -20204,7 +20204,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -20339,9 +20339,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J219"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A140" workbookViewId="0">
+      <selection activeCell="G173" sqref="G173"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="7" max="7" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="97.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="150.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
@@ -20944,7 +20951,7 @@
         <v>11</v>
       </c>
       <c r="G35" t="s">
-        <v>12</v>
+        <v>1481</v>
       </c>
       <c r="H35" t="s">
         <v>11</v>
@@ -21675,7 +21682,7 @@
         <v>11</v>
       </c>
       <c r="G78" t="s">
-        <v>12</v>
+        <v>1481</v>
       </c>
       <c r="H78" t="s">
         <v>11</v>
@@ -21794,7 +21801,7 @@
         <v>11</v>
       </c>
       <c r="G85" t="s">
-        <v>12</v>
+        <v>1481</v>
       </c>
       <c r="H85" t="s">
         <v>11</v>
@@ -23273,7 +23280,7 @@
         <v>11</v>
       </c>
       <c r="G172" t="s">
-        <v>12</v>
+        <v>1481</v>
       </c>
       <c r="H172" t="s">
         <v>11</v>
@@ -24072,7 +24079,7 @@
         <v>11</v>
       </c>
       <c r="G219" t="s">
-        <v>12</v>
+        <v>1481</v>
       </c>
       <c r="H219" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Fixed bug with DFA Highlanders.
</commit_message>
<xml_diff>
--- a/vfProcGenStores/res/test-xlrp-store-content.xlsx
+++ b/vfProcGenStores/res/test-xlrp-store-content.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Bradley T. Burcar\Source\Repos\XLRP-Complete\vfProcGenStores\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{766BF95E-0B93-4665-8DAB-4C3B91957CDD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07199BE0-423A-4578-B3A5-4604947245D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UpgradeDef" sheetId="1" r:id="rId1"/>
@@ -6914,8 +6914,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J183"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -10097,8 +10097,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J466"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -16889,8 +16889,8 @@
     <col min="5" max="5" width="15.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="120.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25" customWidth="1"/>
+    <col min="9" max="9" width="15.44140625" customWidth="1"/>
     <col min="10" max="10" width="121.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -19177,8 +19177,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J382"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
Updates to weapon costs.
</commit_message>
<xml_diff>
--- a/vfProcGenStores/res/test-xlrp-store-content.xlsx
+++ b/vfProcGenStores/res/test-xlrp-store-content.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Bradley T. Burcar\Source\Repos\XLRP-Complete\vfProcGenStores\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07199BE0-423A-4578-B3A5-4604947245D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C31AB923-0AB2-4BB3-A0F9-2A67B1A868AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6914,7 +6914,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J183"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Turret and minor bug fixes.
</commit_message>
<xml_diff>
--- a/vfProcGenStores/res/test-xlrp-store-content.xlsx
+++ b/vfProcGenStores/res/test-xlrp-store-content.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\Steam\steamapps\common\BATTLETECH\Mods\vfProcGenStores\res\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Bradley T. Burcar\Source\Repos\Battletech-Revised\vfProcGenStores\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA4A1EF5-B00E-4FA2-8A0A-E3AFC972D814}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00A0A819-1471-42CF-87CD-C4A92DC14881}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4821,7 +4821,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B93" sqref="B93"/>
+      <selection pane="bottomLeft" activeCell="A130" sqref="A130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4870,20 +4870,20 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="4" customFormat="1">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:10" s="5" customFormat="1">
+      <c r="A2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="4" t="s">
+      <c r="F2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" s="4" t="s">
+      <c r="H2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="5" t="s">
         <v>10</v>
       </c>
     </row>
@@ -4904,20 +4904,20 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="4" customFormat="1">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:10" s="5" customFormat="1">
+      <c r="A4" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="4" t="s">
+      <c r="F4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I4" s="4" t="s">
+      <c r="H4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" s="5" t="s">
         <v>10</v>
       </c>
     </row>
@@ -5271,148 +5271,124 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:9" s="4" customFormat="1">
-      <c r="A27" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H27" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I27" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" s="4" customFormat="1">
-      <c r="A28" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="H28" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I28" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" s="4" customFormat="1">
-      <c r="A29" s="4" t="s">
-        <v>1145</v>
+    <row r="27" spans="1:9" s="5" customFormat="1">
+      <c r="A27" s="5" t="s">
+        <v>1151</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" s="5" customFormat="1">
+      <c r="A28" s="5" t="s">
+        <v>1152</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" s="5" customFormat="1">
+      <c r="A29" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I29" s="5" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:9" s="5" customFormat="1">
       <c r="A30" s="5" t="s">
-        <v>1151</v>
+        <v>66</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="I30" s="5" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:9" s="5" customFormat="1">
       <c r="A31" s="5" t="s">
-        <v>1152</v>
+        <v>67</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H31" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="I31" s="5" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:9" s="5" customFormat="1">
       <c r="A32" s="5" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>10</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="I32" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:9" s="4" customFormat="1">
-      <c r="A33" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G33" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H33" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I33" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" s="4" customFormat="1">
-      <c r="A34" s="4" t="s">
-        <v>1148</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" s="4" customFormat="1">
-      <c r="A35" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="F35" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G35" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H35" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I35" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" s="4" customFormat="1">
-      <c r="A36" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="F36" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G36" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H36" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I36" s="4" t="s">
-        <v>10</v>
+    <row r="33" spans="1:9" s="5" customFormat="1">
+      <c r="A33" s="5" t="s">
+        <v>1153</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" s="5" customFormat="1">
+      <c r="A34" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I34" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" s="5" customFormat="1">
+      <c r="A35" s="5" t="s">
+        <v>1154</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" s="5" customFormat="1">
+      <c r="A36" s="5" t="s">
+        <v>1155</v>
       </c>
     </row>
     <row r="37" spans="1:9" s="5" customFormat="1">
       <c r="A37" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="F37" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G37" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H37" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="I37" s="5" t="s">
-        <v>10</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="38" spans="1:9" s="5" customFormat="1">
       <c r="A38" s="5" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="F38" s="5" t="s">
         <v>10</v>
@@ -5421,7 +5397,7 @@
         <v>38</v>
       </c>
       <c r="H38" s="5" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="I38" s="5" t="s">
         <v>10</v>
@@ -5429,16 +5405,16 @@
     </row>
     <row r="39" spans="1:9" s="5" customFormat="1">
       <c r="A39" s="5" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="F39" s="5" t="s">
         <v>10</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="H39" s="5" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="I39" s="5" t="s">
         <v>10</v>
@@ -5446,21 +5422,33 @@
     </row>
     <row r="40" spans="1:9" s="5" customFormat="1">
       <c r="A40" s="5" t="s">
-        <v>1153</v>
+        <v>74</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H40" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I40" s="5" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="41" spans="1:9" s="5" customFormat="1">
       <c r="A41" s="5" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="F41" s="5" t="s">
         <v>10</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H41" s="5" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="I41" s="5" t="s">
         <v>10</v>
@@ -5468,65 +5456,65 @@
     </row>
     <row r="42" spans="1:9" s="5" customFormat="1">
       <c r="A42" s="5" t="s">
-        <v>1154</v>
+        <v>76</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H42" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="I42" s="5" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="43" spans="1:9" s="5" customFormat="1">
       <c r="A43" s="5" t="s">
-        <v>1155</v>
+        <v>83</v>
+      </c>
+      <c r="F43" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G43" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H43" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I43" s="5" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="44" spans="1:9" s="5" customFormat="1">
       <c r="A44" s="5" t="s">
-        <v>1156</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" s="4" customFormat="1">
-      <c r="A45" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="F45" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G45" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H45" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I45" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" s="4" customFormat="1">
-      <c r="A46" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="F46" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G46" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H46" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I46" s="4" t="s">
-        <v>10</v>
+        <v>1160</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" s="5" customFormat="1">
+      <c r="A45" s="5" t="s">
+        <v>1161</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" s="5" customFormat="1">
+      <c r="A46" s="5" t="s">
+        <v>1162</v>
       </c>
     </row>
     <row r="47" spans="1:9" s="5" customFormat="1">
       <c r="A47" s="5" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="F47" s="5" t="s">
         <v>10</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="H47" s="5" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="I47" s="5" t="s">
         <v>10</v>
@@ -5534,16 +5522,16 @@
     </row>
     <row r="48" spans="1:9" s="5" customFormat="1">
       <c r="A48" s="5" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
       <c r="F48" s="5" t="s">
         <v>10</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="H48" s="5" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="I48" s="5" t="s">
         <v>10</v>
@@ -5551,16 +5539,16 @@
     </row>
     <row r="49" spans="1:9" s="5" customFormat="1">
       <c r="A49" s="5" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="F49" s="5" t="s">
         <v>10</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H49" s="5" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="I49" s="5" t="s">
         <v>10</v>
@@ -5568,7 +5556,7 @@
     </row>
     <row r="50" spans="1:9" s="5" customFormat="1">
       <c r="A50" s="5" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="F50" s="5" t="s">
         <v>10</v>
@@ -5585,13 +5573,13 @@
     </row>
     <row r="51" spans="1:9" s="5" customFormat="1">
       <c r="A51" s="5" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="F51" s="5" t="s">
         <v>10</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="H51" s="5" t="s">
         <v>34</v>
@@ -5600,26 +5588,26 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:9" s="4" customFormat="1">
-      <c r="A52" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="F52" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G52" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="H52" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I52" s="4" t="s">
+    <row r="52" spans="1:9" s="5" customFormat="1">
+      <c r="A52" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G52" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="H52" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="I52" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="53" spans="1:9" s="5" customFormat="1">
       <c r="A53" s="5" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="F53" s="5" t="s">
         <v>10</v>
@@ -5634,99 +5622,147 @@
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="1:9" s="4" customFormat="1">
-      <c r="A54" s="4" t="s">
-        <v>1157</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" s="4" customFormat="1">
-      <c r="A55" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="F55" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G55" s="4" t="s">
+    <row r="54" spans="1:9" s="5" customFormat="1">
+      <c r="A54" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="F54" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G54" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="H54" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="I54" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" s="5" customFormat="1">
+      <c r="A55" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="F55" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G55" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H55" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="I55" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" s="5" customFormat="1">
+      <c r="A56" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="F56" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G56" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H56" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="I56" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" s="5" customFormat="1">
+      <c r="A57" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="F57" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G57" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="H55" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I55" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" s="4" customFormat="1">
-      <c r="A56" s="4" t="s">
-        <v>1158</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" s="4" customFormat="1">
-      <c r="A57" s="4" t="s">
-        <v>1159</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" s="4" customFormat="1">
-      <c r="A58" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="F58" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G58" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="H58" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I58" s="4" t="s">
-        <v>10</v>
+      <c r="H57" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I57" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" s="5" customFormat="1">
+      <c r="A58" s="5" t="s">
+        <v>1147</v>
       </c>
     </row>
     <row r="59" spans="1:9" s="5" customFormat="1">
       <c r="A59" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="F59" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G59" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H59" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I59" s="5" t="s">
-        <v>10</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="60" spans="1:9" s="5" customFormat="1">
       <c r="A60" s="5" t="s">
-        <v>1160</v>
+        <v>99</v>
+      </c>
+      <c r="F60" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G60" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H60" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="I60" s="5" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="61" spans="1:9" s="5" customFormat="1">
       <c r="A61" s="5" t="s">
-        <v>1161</v>
+        <v>100</v>
+      </c>
+      <c r="F61" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G61" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="H61" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="I61" s="5" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="62" spans="1:9" s="5" customFormat="1">
       <c r="A62" s="5" t="s">
-        <v>1162</v>
+        <v>101</v>
+      </c>
+      <c r="F62" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G62" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H62" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="I62" s="5" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="63" spans="1:9" s="5" customFormat="1">
       <c r="A63" s="5" t="s">
-        <v>84</v>
+        <v>102</v>
       </c>
       <c r="F63" s="5" t="s">
         <v>10</v>
       </c>
       <c r="G63" s="5" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="H63" s="5" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="I63" s="5" t="s">
         <v>10</v>
@@ -5734,132 +5770,72 @@
     </row>
     <row r="64" spans="1:9" s="5" customFormat="1">
       <c r="A64" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="F64" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G64" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="H64" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="I64" s="5" t="s">
-        <v>10</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="65" spans="1:9" s="5" customFormat="1">
       <c r="A65" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="F65" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G65" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H65" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="I65" s="5" t="s">
-        <v>10</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="66" spans="1:9" s="5" customFormat="1">
       <c r="A66" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="F66" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G66" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H66" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="I66" s="5" t="s">
-        <v>10</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="67" spans="1:9" s="5" customFormat="1">
       <c r="A67" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="F67" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G67" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="H67" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="I67" s="5" t="s">
-        <v>10</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="68" spans="1:9" s="5" customFormat="1">
       <c r="A68" s="5" t="s">
-        <v>89</v>
+        <v>103</v>
       </c>
       <c r="F68" s="5" t="s">
         <v>10</v>
       </c>
       <c r="G68" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H68" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="I68" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" s="5" customFormat="1">
+      <c r="A69" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="F69" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G69" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="H68" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="I68" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" s="4" customFormat="1">
-      <c r="A69" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="F69" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G69" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H69" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I69" s="4" t="s">
+      <c r="H69" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="I69" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="70" spans="1:9" s="5" customFormat="1">
       <c r="A70" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="F70" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G70" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="H70" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I70" s="5" t="s">
-        <v>10</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="71" spans="1:9" s="5" customFormat="1">
       <c r="A71" s="5" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="F71" s="5" t="s">
         <v>10</v>
       </c>
       <c r="G71" s="5" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="H71" s="5" t="s">
         <v>47</v>
@@ -5870,16 +5846,16 @@
     </row>
     <row r="72" spans="1:9" s="5" customFormat="1">
       <c r="A72" s="5" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="F72" s="5" t="s">
         <v>10</v>
       </c>
       <c r="G72" s="5" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="H72" s="5" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="I72" s="5" t="s">
         <v>10</v>
@@ -5887,94 +5863,82 @@
     </row>
     <row r="73" spans="1:9" s="5" customFormat="1">
       <c r="A73" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="F73" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G73" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H73" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="I73" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" s="4" customFormat="1">
-      <c r="A74" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="F74" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G74" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="H74" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I74" s="4" t="s">
-        <v>10</v>
+        <v>1169</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" s="5" customFormat="1">
+      <c r="A74" s="5" t="s">
+        <v>1170</v>
       </c>
     </row>
     <row r="75" spans="1:9" s="5" customFormat="1">
       <c r="A75" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="F75" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G75" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="H75" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I75" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" s="4" customFormat="1">
-      <c r="A76" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="F76" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G76" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="H76" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I76" s="4" t="s">
+        <v>1171</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" s="5" customFormat="1">
+      <c r="A76" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="F76" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G76" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="H76" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="I76" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="77" spans="1:9" s="5" customFormat="1">
       <c r="A77" s="5" t="s">
-        <v>1147</v>
+        <v>108</v>
+      </c>
+      <c r="F77" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G77" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H77" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="I77" s="5" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="78" spans="1:9" s="5" customFormat="1">
       <c r="A78" s="5" t="s">
-        <v>1163</v>
+        <v>109</v>
+      </c>
+      <c r="F78" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G78" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H78" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="I78" s="5" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="79" spans="1:9" s="5" customFormat="1">
       <c r="A79" s="5" t="s">
-        <v>99</v>
+        <v>110</v>
       </c>
       <c r="F79" s="5" t="s">
         <v>10</v>
       </c>
       <c r="G79" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H79" s="5" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="I79" s="5" t="s">
         <v>10</v>
@@ -5982,16 +5946,16 @@
     </row>
     <row r="80" spans="1:9" s="5" customFormat="1">
       <c r="A80" s="5" t="s">
-        <v>100</v>
+        <v>15</v>
       </c>
       <c r="F80" s="5" t="s">
         <v>10</v>
       </c>
       <c r="G80" s="5" t="s">
-        <v>46</v>
+        <v>11</v>
       </c>
       <c r="H80" s="5" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="I80" s="5" t="s">
         <v>10</v>
@@ -5999,16 +5963,16 @@
     </row>
     <row r="81" spans="1:9" s="5" customFormat="1">
       <c r="A81" s="5" t="s">
-        <v>101</v>
+        <v>16</v>
       </c>
       <c r="F81" s="5" t="s">
         <v>10</v>
       </c>
       <c r="G81" s="5" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="H81" s="5" t="s">
-        <v>47</v>
+        <v>10</v>
       </c>
       <c r="I81" s="5" t="s">
         <v>10</v>
@@ -6016,13 +5980,13 @@
     </row>
     <row r="82" spans="1:9" s="5" customFormat="1">
       <c r="A82" s="5" t="s">
-        <v>102</v>
+        <v>17</v>
       </c>
       <c r="F82" s="5" t="s">
         <v>10</v>
       </c>
       <c r="G82" s="5" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="H82" s="5" t="s">
         <v>10</v>
@@ -6033,279 +5997,315 @@
     </row>
     <row r="83" spans="1:9" s="5" customFormat="1">
       <c r="A83" s="5" t="s">
-        <v>1164</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9" s="5" customFormat="1">
-      <c r="A84" s="5" t="s">
-        <v>1165</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9" s="5" customFormat="1">
-      <c r="A85" s="5" t="s">
-        <v>1166</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9" s="5" customFormat="1">
-      <c r="A86" s="5" t="s">
-        <v>1167</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9" s="5" customFormat="1">
-      <c r="A87" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="F87" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G87" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="H87" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="I87" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9" s="5" customFormat="1">
-      <c r="A88" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="F88" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G88" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="H88" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="I88" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="89" spans="1:9" s="5" customFormat="1">
-      <c r="A89" s="5" t="s">
-        <v>1168</v>
-      </c>
-    </row>
-    <row r="90" spans="1:9" s="5" customFormat="1">
-      <c r="A90" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="F90" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G90" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F83" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G83" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H83" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I83" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" s="4" customFormat="1">
+      <c r="A84" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F84" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G84" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H84" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I84" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" s="4" customFormat="1">
+      <c r="A85" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F85" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G85" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H85" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I85" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" s="4" customFormat="1">
+      <c r="A86" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="F86" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G86" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="H90" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="I90" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="91" spans="1:9" s="5" customFormat="1">
-      <c r="A91" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="F91" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G91" s="5" t="s">
+      <c r="H86" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I86" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" s="4" customFormat="1">
+      <c r="A87" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F87" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G87" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="H91" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I91" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="92" spans="1:9" s="5" customFormat="1">
-      <c r="A92" s="5" t="s">
-        <v>1169</v>
-      </c>
-    </row>
-    <row r="93" spans="1:9" s="5" customFormat="1">
-      <c r="A93" s="5" t="s">
-        <v>1170</v>
-      </c>
-    </row>
-    <row r="94" spans="1:9" s="5" customFormat="1">
-      <c r="A94" s="5" t="s">
-        <v>1171</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9" s="5" customFormat="1">
-      <c r="A95" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="F95" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G95" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="H95" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="I95" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="96" spans="1:9" s="5" customFormat="1">
-      <c r="A96" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="F96" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G96" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="H96" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="I96" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="97" spans="1:9" s="5" customFormat="1">
-      <c r="A97" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="F97" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G97" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="H97" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="I97" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="98" spans="1:9" s="5" customFormat="1">
-      <c r="A98" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="F98" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G98" s="5" t="s">
+      <c r="H87" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I87" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" s="4" customFormat="1">
+      <c r="A88" s="4" t="s">
+        <v>1145</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" s="4" customFormat="1">
+      <c r="A89" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F89" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G89" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H89" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I89" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" s="4" customFormat="1">
+      <c r="A90" s="4" t="s">
+        <v>1148</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" s="4" customFormat="1">
+      <c r="A91" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F91" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G91" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H91" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I91" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" s="4" customFormat="1">
+      <c r="A92" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F92" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G92" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H92" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I92" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" s="4" customFormat="1">
+      <c r="A93" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F93" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G93" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H93" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I93" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" s="4" customFormat="1">
+      <c r="A94" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F94" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G94" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H94" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I94" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" s="4" customFormat="1">
+      <c r="A95" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="F95" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G95" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="H98" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I98" s="5" t="s">
+      <c r="H95" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I95" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" s="4" customFormat="1">
+      <c r="A96" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F96" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G96" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H96" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I96" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" s="4" customFormat="1">
+      <c r="A97" s="4" t="s">
+        <v>1157</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" s="4" customFormat="1">
+      <c r="A98" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F98" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G98" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H98" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I98" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="99" spans="1:9" s="4" customFormat="1">
       <c r="A99" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F99" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G99" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H99" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I99" s="4" t="s">
-        <v>10</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="100" spans="1:9" s="4" customFormat="1">
       <c r="A100" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F100" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G100" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H100" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I100" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="101" spans="1:9" s="5" customFormat="1">
-      <c r="A101" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F101" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G101" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H101" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I101" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="102" spans="1:9" s="5" customFormat="1">
-      <c r="A102" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F102" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G102" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H102" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I102" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="103" spans="1:9" s="5" customFormat="1">
-      <c r="A103" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F103" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G103" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H103" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I103" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="104" spans="1:9" s="5" customFormat="1">
-      <c r="A104" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F104" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G104" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H104" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I104" s="5" t="s">
+        <v>1159</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" s="4" customFormat="1">
+      <c r="A101" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F101" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G101" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H101" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I101" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" s="4" customFormat="1">
+      <c r="A102" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="F102" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G102" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H102" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I102" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" s="4" customFormat="1">
+      <c r="A103" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="F103" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G103" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H103" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I103" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" s="4" customFormat="1">
+      <c r="A104" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="F104" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G104" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H104" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I104" s="4" t="s">
         <v>10</v>
       </c>
     </row>
@@ -6343,71 +6343,71 @@
         <v>10</v>
       </c>
     </row>
-    <row r="107" spans="1:9" s="5" customFormat="1">
-      <c r="A107" s="5" t="s">
+    <row r="107" spans="1:9" s="4" customFormat="1">
+      <c r="A107" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F107" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G107" s="5" t="s">
+      <c r="F107" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G107" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H107" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I107" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="108" spans="1:9" s="5" customFormat="1">
-      <c r="A108" s="5" t="s">
+      <c r="H107" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I107" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" s="4" customFormat="1">
+      <c r="A108" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F108" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G108" s="5" t="s">
+      <c r="F108" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G108" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H108" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I108" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="109" spans="1:9" s="5" customFormat="1">
-      <c r="A109" s="5" t="s">
+      <c r="H108" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I108" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" s="4" customFormat="1">
+      <c r="A109" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F109" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G109" s="5" t="s">
+      <c r="F109" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G109" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H109" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I109" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="110" spans="1:9" s="5" customFormat="1">
-      <c r="A110" s="5" t="s">
+      <c r="H109" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I109" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" s="4" customFormat="1">
+      <c r="A110" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F110" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G110" s="5" t="s">
+      <c r="F110" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G110" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H110" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I110" s="5" t="s">
+      <c r="H110" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I110" s="4" t="s">
         <v>10</v>
       </c>
     </row>
@@ -6462,20 +6462,20 @@
         <v>10</v>
       </c>
     </row>
-    <row r="114" spans="1:9" s="5" customFormat="1">
-      <c r="A114" s="5" t="s">
+    <row r="114" spans="1:9" s="4" customFormat="1">
+      <c r="A114" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="F114" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G114" s="5" t="s">
+      <c r="F114" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G114" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="H114" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I114" s="5" t="s">
+      <c r="H114" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I114" s="4" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>